<commit_message>
Mise à jour journal TA
</commit_message>
<xml_diff>
--- a/LM_Journal_Travail.xlsx
+++ b/LM_Journal_Travail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmes\VS2019\Projets\Projet Gerber\Love-Mirroring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositories\Love-Mirroring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A221DC9D-07F9-4167-9A55-F253FBA85652}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C764AA62-7677-4028-9073-B1D2F2881C20}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
     <definedName name="NBLecons">#REF!</definedName>
     <definedName name="TachesPlanifiees">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5770,7 +5770,7 @@
   <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6063,7 +6063,7 @@
         <v>23</v>
       </c>
       <c r="B11" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="12" t="s">
@@ -6089,7 +6089,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="12" t="s">

</xml_diff>